<commit_message>
Ajout des éléments de conception détaillée et de données.
</commit_message>
<xml_diff>
--- a/TP05/documents/Moodle/Form données de projet.xlsx
+++ b/TP05/documents/Moodle/Form données de projet.xlsx
@@ -1778,9 +1778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1940,7 +1940,7 @@
         <v>130</v>
       </c>
       <c r="J4" s="21">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="K4" s="21">
         <v>0</v>
@@ -1993,7 +1993,7 @@
         <v>11</v>
       </c>
       <c r="J5" s="21">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="21">
         <v>0</v>
@@ -2046,7 +2046,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6" s="21">
         <v>0</v>
@@ -2101,7 +2101,7 @@
         <v>67</v>
       </c>
       <c r="J7" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K7" s="21">
         <v>0</v>
@@ -2157,7 +2157,7 @@
         <v>130</v>
       </c>
       <c r="J8" s="21">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K8" s="21">
         <v>0</v>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="R8" s="4">
         <f>D8+F8+H8+J8+L8+N8+P8</f>
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="S8" s="18"/>
       <c r="T8" s="4">
@@ -2219,7 +2219,7 @@
         <v>77</v>
       </c>
       <c r="J9" s="21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K9" s="21">
         <v>0</v>
@@ -2250,7 +2250,7 @@
       </c>
       <c r="R9" s="4">
         <f>D9+F9+H9+J9+L9+N9+P9</f>
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="S9" s="18"/>
       <c r="T9" s="4">
@@ -2287,7 +2287,7 @@
         <v>244</v>
       </c>
       <c r="J10" s="21">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="K10" s="21">
         <v>0</v>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="R10" s="4">
         <f>D10+F10+H10+J10+L10+N10+P10</f>
-        <v>412</v>
+        <v>541</v>
       </c>
       <c r="S10" s="18"/>
       <c r="T10" s="4">
@@ -2486,7 +2486,7 @@
         <v>45</v>
       </c>
       <c r="J14" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K14" s="21">
         <v>0</v>
@@ -2511,11 +2511,11 @@
       </c>
       <c r="R14" s="4">
         <f t="shared" ref="R14:R23" si="2">D14+F14+H14+J14+L14+N14+P14</f>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="S14" s="19">
         <f t="shared" ref="S14:S23" si="3">R14/$R$24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>8.3916083916083919E-2</v>
       </c>
       <c r="T14" s="4">
         <f t="shared" si="1"/>
@@ -2555,7 +2555,7 @@
         <v>60</v>
       </c>
       <c r="J15" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K15" s="21">
         <v>0</v>
@@ -2580,11 +2580,11 @@
       </c>
       <c r="R15" s="4">
         <f t="shared" si="2"/>
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="S15" s="19">
         <f t="shared" si="3"/>
-        <v>0.13333333333333333</v>
+        <v>0.12587412587412589</v>
       </c>
       <c r="T15" s="4">
         <f t="shared" si="1"/>
@@ -2620,7 +2620,7 @@
         <v>30</v>
       </c>
       <c r="J16" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K16" s="21">
         <v>0</v>
@@ -2645,11 +2645,11 @@
       </c>
       <c r="R16" s="4">
         <f t="shared" si="2"/>
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="S16" s="19">
         <f t="shared" si="3"/>
-        <v>0.13333333333333333</v>
+        <v>0.12587412587412589</v>
       </c>
       <c r="T16" s="4">
         <f t="shared" si="1"/>
@@ -2689,7 +2689,7 @@
         <v>120</v>
       </c>
       <c r="J17" s="21">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K17" s="21">
         <v>0</v>
@@ -2714,11 +2714,11 @@
       </c>
       <c r="R17" s="4">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="S17" s="19">
         <f t="shared" si="3"/>
-        <v>0.16666666666666666</v>
+        <v>0.16783216783216784</v>
       </c>
       <c r="T17" s="4">
         <f t="shared" si="1"/>
@@ -2754,7 +2754,7 @@
         <v>60</v>
       </c>
       <c r="J18" s="21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K18" s="21">
         <v>0</v>
@@ -2779,11 +2779,11 @@
       </c>
       <c r="R18" s="4">
         <f t="shared" si="2"/>
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="S18" s="19">
         <f t="shared" si="3"/>
-        <v>0.11666666666666667</v>
+        <v>0.1048951048951049</v>
       </c>
       <c r="T18" s="4">
         <f t="shared" si="1"/>
@@ -2823,7 +2823,7 @@
         <v>45</v>
       </c>
       <c r="J19" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K19" s="21">
         <v>0</v>
@@ -2848,11 +2848,11 @@
       </c>
       <c r="R19" s="4">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="S19" s="19">
         <f t="shared" si="3"/>
-        <v>0.16666666666666666</v>
+        <v>0.16083916083916083</v>
       </c>
       <c r="T19" s="4">
         <f t="shared" si="1"/>
@@ -2888,7 +2888,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K20" s="21">
         <v>0</v>
@@ -2913,11 +2913,11 @@
       </c>
       <c r="R20" s="4">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="S20" s="19">
         <f t="shared" si="3"/>
-        <v>1.1111111111111112E-2</v>
+        <v>2.3310023310023312E-2</v>
       </c>
       <c r="T20" s="4">
         <f t="shared" si="1"/>
@@ -2945,7 +2945,7 @@
         <v>10</v>
       </c>
       <c r="J21" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K21" s="21">
         <v>0</v>
@@ -2970,11 +2970,11 @@
       </c>
       <c r="R21" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="S21" s="19">
         <f t="shared" si="3"/>
-        <v>5.5555555555555558E-3</v>
+        <v>1.8648018648018648E-2</v>
       </c>
       <c r="T21" s="4">
         <f t="shared" si="1"/>
@@ -3010,7 +3010,7 @@
         <v>30</v>
       </c>
       <c r="J22" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K22" s="21">
         <v>0</v>
@@ -3035,11 +3035,11 @@
       </c>
       <c r="R22" s="4">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="S22" s="19">
         <f t="shared" si="3"/>
-        <v>8.3333333333333329E-2</v>
+        <v>8.3916083916083919E-2</v>
       </c>
       <c r="T22" s="4">
         <f t="shared" si="1"/>
@@ -3079,7 +3079,7 @@
         <v>30</v>
       </c>
       <c r="J23" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K23" s="21">
         <v>0</v>
@@ -3104,11 +3104,11 @@
       </c>
       <c r="R23" s="4">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="S23" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.1048951048951049</v>
       </c>
       <c r="T23" s="4">
         <f t="shared" si="1"/>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="J24" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="K24" s="9">
         <f t="shared" si="5"/>
@@ -3189,11 +3189,11 @@
       </c>
       <c r="R24" s="10">
         <f>SUM(R13:R23)</f>
-        <v>1800</v>
+        <v>2145</v>
       </c>
       <c r="S24" s="11">
         <f>SUM(S13:S23)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="T24" s="10">
         <f>SUM(T13:T23)</f>
@@ -3291,9 +3291,9 @@
         <f t="shared" ref="R26:R36" si="8">D26+F26+H26+J26+L26+N26+P26</f>
         <v>0</v>
       </c>
-      <c r="S26" s="19" t="e">
+      <c r="S26" s="19">
         <f>R26/$R$37</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T26" s="4">
         <f t="shared" ref="T26:T36" si="9">E26+G26+I26+K26+M26+O26+Q26</f>
@@ -3358,9 +3358,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S27" s="19" t="e">
+      <c r="S27" s="19">
         <f t="shared" ref="S27:S36" si="10">R27/$R$37</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T27" s="4">
         <f t="shared" si="9"/>
@@ -3425,9 +3425,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S28" s="19" t="e">
+      <c r="S28" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T28" s="4">
         <f t="shared" si="9"/>
@@ -3490,9 +3490,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S29" s="19" t="e">
+      <c r="S29" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T29" s="4">
         <f t="shared" si="9"/>
@@ -3557,9 +3557,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S30" s="19" t="e">
+      <c r="S30" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T30" s="4">
         <f t="shared" si="9"/>
@@ -3595,7 +3595,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K31" s="21">
         <v>0</v>
@@ -3620,11 +3620,11 @@
       </c>
       <c r="R31" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="S31" s="19" t="e">
+        <v>2</v>
+      </c>
+      <c r="S31" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="T31" s="4">
         <f t="shared" si="9"/>
@@ -3689,9 +3689,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S32" s="19" t="e">
+      <c r="S32" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T32" s="4">
         <f t="shared" si="9"/>
@@ -3746,9 +3746,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S33" s="19" t="e">
+      <c r="S33" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T33" s="4">
         <f t="shared" si="9"/>
@@ -3801,9 +3801,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S34" s="19" t="e">
+      <c r="S34" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T34" s="4">
         <f t="shared" si="9"/>
@@ -3866,9 +3866,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S35" s="19" t="e">
+      <c r="S35" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T35" s="4">
         <f t="shared" si="9"/>
@@ -3933,9 +3933,9 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S36" s="19" t="e">
+      <c r="S36" s="19">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T36" s="4">
         <f t="shared" si="9"/>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="J37" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K37" s="8">
         <f t="shared" si="12"/>
@@ -4013,11 +4013,11 @@
       </c>
       <c r="R37" s="10">
         <f>SUM(R26:R36)</f>
-        <v>0</v>
-      </c>
-      <c r="S37" s="11" t="e">
+        <v>2</v>
+      </c>
+      <c r="S37" s="11">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="T37" s="10">
         <f>SUM(T26:T36)</f>
@@ -4107,9 +4107,9 @@
         <f t="shared" ref="R39:R49" si="15">D39+F39+H39+J39+L39+N39+P39</f>
         <v>0</v>
       </c>
-      <c r="S39" s="19" t="e">
+      <c r="S39" s="19">
         <f>R39/$R$50</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T39" s="4">
         <f t="shared" ref="T39:T49" si="16">E39+G39+I39+K39+M39+O39+Q39</f>
@@ -4174,9 +4174,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S40" s="19" t="e">
+      <c r="S40" s="19">
         <f t="shared" ref="S40:S49" si="17">R40/$R$50</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T40" s="4">
         <f t="shared" si="16"/>
@@ -4241,9 +4241,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S41" s="19" t="e">
+      <c r="S41" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T41" s="4">
         <f t="shared" si="16"/>
@@ -4306,9 +4306,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S42" s="19" t="e">
+      <c r="S42" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T42" s="4">
         <f t="shared" si="16"/>
@@ -4371,9 +4371,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S43" s="19" t="e">
+      <c r="S43" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T43" s="4">
         <f t="shared" si="16"/>
@@ -4436,9 +4436,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S44" s="19" t="e">
+      <c r="S44" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T44" s="4">
         <f t="shared" si="16"/>
@@ -4476,7 +4476,7 @@
         <v>2</v>
       </c>
       <c r="J45" s="21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K45" s="21">
         <v>0</v>
@@ -4501,11 +4501,11 @@
       </c>
       <c r="R45" s="4">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="S45" s="19" t="e">
+        <v>2</v>
+      </c>
+      <c r="S45" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="T45" s="4">
         <f t="shared" si="16"/>
@@ -4560,9 +4560,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S46" s="19" t="e">
+      <c r="S46" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T46" s="4">
         <f t="shared" si="16"/>
@@ -4617,9 +4617,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S47" s="19" t="e">
+      <c r="S47" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T47" s="4">
         <f t="shared" si="16"/>
@@ -4682,9 +4682,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S48" s="19" t="e">
+      <c r="S48" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T48" s="4">
         <f t="shared" si="16"/>
@@ -4749,9 +4749,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="S49" s="19" t="e">
+      <c r="S49" s="19">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="T49" s="4">
         <f t="shared" si="16"/>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="J50" s="8">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K50" s="8">
         <f t="shared" si="19"/>
@@ -4829,11 +4829,11 @@
       </c>
       <c r="R50" s="10">
         <f>SUM(R39:R49)</f>
-        <v>0</v>
-      </c>
-      <c r="S50" s="11" t="e">
+        <v>2</v>
+      </c>
+      <c r="S50" s="11">
         <f>SUM(S39:S49)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="T50" s="10">
         <f>SUM(T39:T49)</f>
@@ -4918,9 +4918,9 @@
         <f t="shared" si="22"/>
         <v>0.54222222222222227</v>
       </c>
-      <c r="J53" s="22" t="e">
+      <c r="J53" s="22">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
+        <v>0.37391304347826088</v>
       </c>
       <c r="K53" s="22" t="e">
         <f t="shared" si="22"/>
@@ -4985,9 +4985,9 @@
         <f t="shared" si="23"/>
         <v>0.1711111111111111</v>
       </c>
-      <c r="J54" s="22" t="e">
+      <c r="J54" s="22">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="K54" s="22" t="e">
         <f t="shared" si="23"/>
@@ -5066,9 +5066,9 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="J56" s="16"/>
-      <c r="K56" s="22" t="e">
+      <c r="K56" s="22">
         <f>K24/J24</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L56" s="16"/>
       <c r="M56" s="22" t="e">
@@ -5112,9 +5112,9 @@
         <v>1.0124481327800829</v>
       </c>
       <c r="J57" s="16"/>
-      <c r="K57" s="22" t="e">
+      <c r="K57" s="22">
         <f>K10/J10</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L57" s="16"/>
       <c r="M57" s="22" t="e">
@@ -5158,9 +5158,9 @@
         <v>0.96250000000000002</v>
       </c>
       <c r="J58" s="16"/>
-      <c r="K58" s="22" t="e">
+      <c r="K58" s="22">
         <f>K9/J9</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L58" s="16"/>
       <c r="M58" s="22" t="e">
@@ -5259,9 +5259,9 @@
         <f t="shared" si="24"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J61" s="22" t="e">
+      <c r="J61" s="22">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>5.7971014492753624E-3</v>
       </c>
       <c r="K61" s="22" t="e">
         <f t="shared" si="24"/>
@@ -5326,9 +5326,9 @@
         <f t="shared" si="25"/>
         <v>4.4444444444444444E-3</v>
       </c>
-      <c r="J62" s="22" t="e">
+      <c r="J62" s="22">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K62" s="22" t="e">
         <f t="shared" si="25"/>
@@ -5460,9 +5460,9 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="J64" s="22" t="e">
+      <c r="J64" s="22">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K64" s="22" t="e">
         <f t="shared" si="27"/>
@@ -5527,9 +5527,9 @@
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="J65" s="22" t="e">
+      <c r="J65" s="22">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K65" s="22" t="e">
         <f t="shared" si="28"/>
@@ -5594,9 +5594,9 @@
         <f t="shared" si="29"/>
         <v>6.6666666666666671E-3</v>
       </c>
-      <c r="J66" s="22" t="e">
+      <c r="J66" s="22">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K66" s="22" t="e">
         <f t="shared" si="29"/>
@@ -5661,9 +5661,9 @@
         <f t="shared" si="30"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J67" s="22" t="e">
+      <c r="J67" s="22">
         <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K67" s="22" t="e">
         <f t="shared" si="30"/>
@@ -5751,9 +5751,9 @@
         <f t="shared" si="31"/>
         <v>2.0491803278688523E-2</v>
       </c>
-      <c r="J69" s="22" t="e">
+      <c r="J69" s="22">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
+        <v>1.5503875968992248E-2</v>
       </c>
       <c r="K69" s="22" t="e">
         <f t="shared" si="31"/>
@@ -5818,9 +5818,9 @@
         <f t="shared" si="32"/>
         <v>0.1711111111111111</v>
       </c>
-      <c r="J70" s="22" t="e">
+      <c r="J70" s="22">
         <f t="shared" si="32"/>
-        <v>#DIV/0!</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="K70" s="22" t="e">
         <f t="shared" si="32"/>
@@ -5885,9 +5885,9 @@
         <f t="shared" si="33"/>
         <v>1.2295081967213115E-2</v>
       </c>
-      <c r="J71" s="22" t="e">
+      <c r="J71" s="22">
         <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K71" s="22" t="e">
         <f t="shared" si="33"/>
@@ -5952,9 +5952,9 @@
         <f t="shared" si="34"/>
         <v>3.896103896103896E-2</v>
       </c>
-      <c r="J72" s="22" t="e">
+      <c r="J72" s="22">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K72" s="22" t="e">
         <f t="shared" si="34"/>
@@ -6066,9 +6066,9 @@
         <f t="shared" si="35"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J75" s="22" t="e">
+      <c r="J75" s="22">
         <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
+        <v>5.7971014492753624E-3</v>
       </c>
       <c r="K75" s="22" t="e">
         <f t="shared" si="35"/>
@@ -6133,9 +6133,9 @@
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="J76" s="22" t="e">
+      <c r="J76" s="22">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K76" s="22" t="e">
         <f t="shared" si="36"/>
@@ -6200,9 +6200,9 @@
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="J77" s="22" t="e">
+      <c r="J77" s="22">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K77" s="22" t="e">
         <f t="shared" si="37"/>
@@ -6267,9 +6267,9 @@
         <f t="shared" si="38"/>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="J78" s="22" t="e">
+      <c r="J78" s="22">
         <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="K78" s="22" t="e">
         <f t="shared" si="38"/>
@@ -6332,9 +6332,9 @@
         <f t="shared" si="39"/>
         <v>0.1</v>
       </c>
-      <c r="J79" s="23" t="e">
+      <c r="J79" s="23">
         <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K79" s="23" t="e">
         <f t="shared" si="39"/>
@@ -6393,9 +6393,9 @@
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="J80" s="23" t="e">
+      <c r="J80" s="23">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K80" s="23" t="e">
         <f t="shared" si="40"/>
@@ -6454,9 +6454,9 @@
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="J81" s="23" t="e">
+      <c r="J81" s="23">
         <f t="shared" si="41"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K81" s="23" t="e">
         <f t="shared" si="41"/>

</xml_diff>

<commit_message>
ajouts de la phase TEST1 dans le form de données de projet
</commit_message>
<xml_diff>
--- a/TP05/documents/Moodle/Form données de projet.xlsx
+++ b/TP05/documents/Moodle/Form données de projet.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1778,9 +1778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2432,7 +2432,7 @@
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="21">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="L13" s="16"/>
       <c r="M13" s="17">
@@ -2450,11 +2450,11 @@
       <c r="S13" s="19"/>
       <c r="T13" s="4">
         <f t="shared" ref="T13:T23" si="1">E13+G13+I13+K13+M13+O13+Q13</f>
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="U13" s="19">
         <f>T13/$T$24</f>
-        <v>6.9767441860465115E-2</v>
+        <v>9.4043887147335428E-2</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2489,7 +2489,7 @@
         <v>30</v>
       </c>
       <c r="K14" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L14" s="17">
         <v>0</v>
@@ -2519,11 +2519,11 @@
       </c>
       <c r="T14" s="4">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="U14" s="19">
         <f t="shared" ref="U14:U23" si="4">T14/$T$24</f>
-        <v>8.1395348837209308E-2</v>
+        <v>8.4639498432601878E-2</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>30</v>
       </c>
       <c r="K15" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L15" s="17">
         <v>0</v>
@@ -2588,11 +2588,11 @@
       </c>
       <c r="T15" s="4">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="U15" s="19">
         <f t="shared" si="4"/>
-        <v>0.11627906976744186</v>
+        <v>0.11285266457680251</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2623,7 +2623,7 @@
         <v>30</v>
       </c>
       <c r="K16" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L16" s="17">
         <v>0</v>
@@ -2653,11 +2653,11 @@
       </c>
       <c r="T16" s="4">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="U16" s="19">
         <f t="shared" si="4"/>
-        <v>0.11627906976744186</v>
+        <v>0.11285266457680251</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
         <v>60</v>
       </c>
       <c r="K17" s="21">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="L17" s="17">
         <v>0</v>
@@ -2722,11 +2722,11 @@
       </c>
       <c r="T17" s="4">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>315</v>
       </c>
       <c r="U17" s="19">
         <f t="shared" si="4"/>
-        <v>0.18604651162790697</v>
+        <v>0.19749216300940439</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>15</v>
       </c>
       <c r="K18" s="21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L18" s="17">
         <v>0</v>
@@ -2787,11 +2787,11 @@
       </c>
       <c r="T18" s="4">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="U18" s="19">
         <f t="shared" si="4"/>
-        <v>0.13953488372093023</v>
+        <v>0.12225705329153605</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>45</v>
       </c>
       <c r="K19" s="21">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L19" s="17">
         <v>0</v>
@@ -2856,11 +2856,11 @@
       </c>
       <c r="T19" s="4">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="U19" s="19">
         <f t="shared" si="4"/>
-        <v>0.10465116279069768</v>
+        <v>0.11285266457680251</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>30</v>
       </c>
       <c r="K20" s="21">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L20" s="17">
         <v>0</v>
@@ -2921,11 +2921,11 @@
       </c>
       <c r="T20" s="4">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="U20" s="19">
         <f t="shared" si="4"/>
-        <v>1.5503875968992248E-2</v>
+        <v>2.0062695924764892E-2</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>30</v>
       </c>
       <c r="K21" s="21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L21" s="17">
         <v>0</v>
@@ -2978,11 +2978,11 @@
       </c>
       <c r="T21" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="U21" s="19">
         <f t="shared" si="4"/>
-        <v>7.7519379844961239E-3</v>
+        <v>1.128526645768025E-2</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="U22" s="19">
         <f t="shared" si="4"/>
-        <v>9.3023255813953487E-2</v>
+        <v>7.5235109717868343E-2</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="U23" s="19">
         <f t="shared" si="4"/>
-        <v>6.9767441860465115E-2</v>
+        <v>5.6426332288401257E-2</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="K24" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="L24" s="8">
         <f t="shared" ref="L24:O24" si="7">SUM(L13:L23)</f>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="T24" s="10">
         <f>SUM(T13:T23)</f>
-        <v>1290</v>
+        <v>1595</v>
       </c>
       <c r="U24" s="11">
         <f>SUM(U13:U23)</f>
@@ -4922,9 +4922,9 @@
         <f t="shared" si="22"/>
         <v>0.37391304347826088</v>
       </c>
-      <c r="K53" s="22" t="e">
+      <c r="K53" s="22">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L53" s="22" t="e">
         <f t="shared" si="22"/>
@@ -4989,9 +4989,9 @@
         <f t="shared" si="23"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="K54" s="22" t="e">
+      <c r="K54" s="22">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L54" s="22" t="e">
         <f t="shared" si="23"/>
@@ -5068,7 +5068,7 @@
       <c r="J56" s="16"/>
       <c r="K56" s="22">
         <f>K24/J24</f>
-        <v>0</v>
+        <v>0.88405797101449279</v>
       </c>
       <c r="L56" s="16"/>
       <c r="M56" s="22" t="e">
@@ -5263,9 +5263,9 @@
         <f t="shared" si="24"/>
         <v>5.7971014492753624E-3</v>
       </c>
-      <c r="K61" s="22" t="e">
+      <c r="K61" s="22">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L61" s="22" t="e">
         <f t="shared" si="24"/>
@@ -5330,9 +5330,9 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="K62" s="22" t="e">
+      <c r="K62" s="22">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L62" s="22" t="e">
         <f t="shared" si="25"/>
@@ -5397,9 +5397,9 @@
         <f t="shared" si="26"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K63" s="22" t="e">
+      <c r="K63" s="22">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L63" s="22" t="e">
         <f t="shared" si="26"/>
@@ -5464,9 +5464,9 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="K64" s="22" t="e">
+      <c r="K64" s="22">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L64" s="22" t="e">
         <f t="shared" si="27"/>
@@ -5531,9 +5531,9 @@
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="K65" s="22" t="e">
+      <c r="K65" s="22">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L65" s="22" t="e">
         <f t="shared" si="28"/>
@@ -5598,9 +5598,9 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="K66" s="22" t="e">
+      <c r="K66" s="22">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L66" s="22" t="e">
         <f t="shared" si="29"/>
@@ -5665,9 +5665,9 @@
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="K67" s="22" t="e">
+      <c r="K67" s="22">
         <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L67" s="22" t="e">
         <f t="shared" si="30"/>
@@ -5822,9 +5822,9 @@
         <f t="shared" si="32"/>
         <v>4.3478260869565216E-2</v>
       </c>
-      <c r="K70" s="22" t="e">
+      <c r="K70" s="22">
         <f t="shared" si="32"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L70" s="22" t="e">
         <f t="shared" si="32"/>
@@ -6070,9 +6070,9 @@
         <f t="shared" si="35"/>
         <v>5.7971014492753624E-3</v>
       </c>
-      <c r="K75" s="22" t="e">
+      <c r="K75" s="22">
         <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L75" s="22" t="e">
         <f t="shared" si="35"/>
@@ -6137,9 +6137,9 @@
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="K76" s="22" t="e">
+      <c r="K76" s="22">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L76" s="22" t="e">
         <f t="shared" si="36"/>
@@ -6204,9 +6204,9 @@
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="K77" s="22" t="e">
+      <c r="K77" s="22">
         <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L77" s="22" t="e">
         <f t="shared" si="37"/>
@@ -6271,9 +6271,9 @@
         <f t="shared" si="38"/>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="K78" s="22" t="e">
+      <c r="K78" s="22">
         <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L78" s="22" t="e">
         <f t="shared" si="38"/>
@@ -6336,9 +6336,9 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="K79" s="23" t="e">
+      <c r="K79" s="23">
         <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L79" s="23" t="e">
         <f t="shared" si="39"/>
@@ -6397,9 +6397,9 @@
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="K80" s="23" t="e">
+      <c r="K80" s="23">
         <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L80" s="23" t="e">
         <f t="shared" si="40"/>

</xml_diff>

<commit_message>
Reajustement du form de donnees pour Bilan
</commit_message>
<xml_diff>
--- a/TP05/documents/Moodle/Form données de projet.xlsx
+++ b/TP05/documents/Moodle/Form données de projet.xlsx
@@ -1779,8 +1779,8 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="U13" s="19">
         <f>T13/$T$24</f>
-        <v>8.9820359281437126E-2</v>
+        <v>9.036144578313253E-2</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2523,7 +2523,7 @@
       </c>
       <c r="U14" s="19">
         <f t="shared" ref="U14:U23" si="4">T14/$T$24</f>
-        <v>8.0838323353293412E-2</v>
+        <v>8.1325301204819275E-2</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="U15" s="19">
         <f t="shared" si="4"/>
-        <v>0.10778443113772455</v>
+        <v>0.10843373493975904</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="U16" s="19">
         <f t="shared" si="4"/>
-        <v>0.10778443113772455</v>
+        <v>0.10843373493975904</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="U17" s="19">
         <f t="shared" si="4"/>
-        <v>0.18862275449101795</v>
+        <v>0.18975903614457831</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="U18" s="19">
         <f t="shared" si="4"/>
-        <v>0.11676646706586827</v>
+        <v>0.11746987951807229</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="U19" s="19">
         <f t="shared" si="4"/>
-        <v>0.10778443113772455</v>
+        <v>0.10843373493975904</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="U20" s="19">
         <f t="shared" si="4"/>
-        <v>1.9161676646706587E-2</v>
+        <v>1.9277108433734941E-2</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2982,7 +2982,7 @@
       </c>
       <c r="U21" s="19">
         <f t="shared" si="4"/>
-        <v>1.0778443113772455E-2</v>
+        <v>1.0843373493975903E-2</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="U22" s="19">
         <f t="shared" si="4"/>
-        <v>9.880239520958084E-2</v>
+        <v>9.9397590361445784E-2</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3082,7 +3082,7 @@
         <v>45</v>
       </c>
       <c r="K23" s="21">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L23" s="17">
         <v>0</v>
@@ -3112,11 +3112,11 @@
       </c>
       <c r="T23" s="4">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="U23" s="19">
         <f t="shared" si="4"/>
-        <v>7.1856287425149698E-2</v>
+        <v>6.6265060240963861E-2</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="K24" s="9">
         <f t="shared" si="5"/>
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="L24" s="8">
         <f t="shared" ref="L24:O24" si="7">SUM(L13:L23)</f>
@@ -3197,11 +3197,11 @@
       </c>
       <c r="T24" s="10">
         <f>SUM(T13:T23)</f>
-        <v>1670</v>
+        <v>1660</v>
       </c>
       <c r="U24" s="11">
         <f>SUM(U13:U23)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="K53" s="22">
         <f t="shared" si="22"/>
-        <v>0.48157894736842105</v>
+        <v>0.49459459459459459</v>
       </c>
       <c r="L53" s="22" t="e">
         <f t="shared" si="22"/>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="K54" s="22">
         <f t="shared" si="23"/>
-        <v>8.9473684210526316E-2</v>
+        <v>9.1891891891891897E-2</v>
       </c>
       <c r="L54" s="22" t="e">
         <f t="shared" si="23"/>
@@ -5068,7 +5068,7 @@
       <c r="J56" s="16"/>
       <c r="K56" s="22">
         <f>K24/J24</f>
-        <v>1.1014492753623188</v>
+        <v>1.0724637681159421</v>
       </c>
       <c r="L56" s="16"/>
       <c r="M56" s="22" t="e">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="K61" s="22">
         <f t="shared" si="24"/>
-        <v>1.0526315789473684E-2</v>
+        <v>1.0810810810810811E-2</v>
       </c>
       <c r="L61" s="22" t="e">
         <f t="shared" si="24"/>
@@ -5824,7 +5824,7 @@
       </c>
       <c r="K70" s="22">
         <f t="shared" si="32"/>
-        <v>8.9473684210526316E-2</v>
+        <v>9.1891891891891897E-2</v>
       </c>
       <c r="L70" s="22" t="e">
         <f t="shared" si="32"/>
@@ -6072,7 +6072,7 @@
       </c>
       <c r="K75" s="22">
         <f t="shared" si="35"/>
-        <v>1.0526315789473684E-2</v>
+        <v>1.0810810810810811E-2</v>
       </c>
       <c r="L75" s="22" t="e">
         <f t="shared" si="35"/>

</xml_diff>